<commit_message>
Modified and created cfu_data.xlsx added new ID variable created Rmd and started analysis
</commit_message>
<xml_diff>
--- a/raw_files/cfu_actinobacteria.xlsx
+++ b/raw_files/cfu_actinobacteria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raquel.correa\Desktop\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.romero\ownCloud - Romero Ignacio@owncloud.fibl.org\exchange_iro_nbo_vgf\iro\banana_microbiome\raw_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C997B20-F3BC-481F-A819-3CBA069543B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55B390-6A6C-4078-B2F7-1A72C189B1A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{65FEA12C-D4E3-4D9D-BB5A-CCA2AEA21078}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{65FEA12C-D4E3-4D9D-BB5A-CCA2AEA21078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="18">
   <si>
     <t>time</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>control.legumes</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>actinobacteria</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>exp.id</t>
   </si>
 </sst>
 </file>
@@ -427,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6965D11-17F6-4B89-8430-518B48E14CEB}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +457,17 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -456,8 +477,18 @@
       <c r="C2">
         <v>83500</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>A2&amp;"_"&amp;B2&amp;"_"&amp;"actino"&amp;"_"&amp;E2</f>
+        <v>t0_control_actino_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -467,8 +498,18 @@
       <c r="C3">
         <v>25500</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">A3&amp;"_"&amp;B3&amp;"_"&amp;"actino"&amp;"_"&amp;E3</f>
+        <v>t0_control_actino_2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -478,8 +519,18 @@
       <c r="C4">
         <v>11000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control_actino_3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -489,8 +540,18 @@
       <c r="C5">
         <v>70500</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.amf_actino_1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -500,8 +561,18 @@
       <c r="C6">
         <v>38000</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.amf_actino_2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -511,8 +582,18 @@
       <c r="C7">
         <v>12500</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.amf_actino_3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -522,8 +603,18 @@
       <c r="C8">
         <v>350000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_chicken.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -533,8 +624,18 @@
       <c r="C9">
         <v>2380000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_chicken.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -544,8 +645,18 @@
       <c r="C10">
         <v>840000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_chicken.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -555,8 +666,18 @@
       <c r="C11">
         <v>595000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_cow.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -566,8 +687,18 @@
       <c r="C12">
         <v>58500</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_cow.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -577,8 +708,18 @@
       <c r="C13">
         <v>385000</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_cow.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -588,8 +729,18 @@
       <c r="C14">
         <v>119000</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_mo.pellet_actino_1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -599,8 +750,18 @@
       <c r="C15">
         <v>38000</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_mo.pellet_actino_2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -610,8 +771,18 @@
       <c r="C16">
         <v>72500</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_mo.pellet_actino_3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -621,8 +792,18 @@
       <c r="C17">
         <v>950000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_compost_actino_1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -632,8 +813,18 @@
       <c r="C18">
         <v>935000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_compost_actino_2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -643,8 +834,18 @@
       <c r="C19">
         <v>725000</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_compost_actino_3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -654,8 +855,18 @@
       <c r="C20">
         <v>83000</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.legumes_actino_1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -665,8 +876,18 @@
       <c r="C21">
         <v>52000</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.legumes_actino_2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -676,8 +897,18 @@
       <c r="C22">
         <v>18000</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>t0_control.legumes_actino_3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -687,8 +918,18 @@
       <c r="C23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>time_treatment_actino_1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -698,8 +939,18 @@
       <c r="C24">
         <v>65000</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control_actino_2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -709,8 +960,18 @@
       <c r="C25">
         <v>46500</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control_actino_3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -720,8 +981,18 @@
       <c r="C26">
         <v>83500</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control_actino_1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -731,8 +1002,18 @@
       <c r="C27">
         <v>49500</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.amf_actino_2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -742,8 +1023,18 @@
       <c r="C28">
         <v>53500</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.amf_actino_3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -753,8 +1044,18 @@
       <c r="C29">
         <v>45500</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.amf_actino_1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -764,8 +1065,18 @@
       <c r="C30">
         <v>44500</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_chicken.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -775,8 +1086,18 @@
       <c r="C31">
         <v>1400000</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_chicken.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -786,8 +1107,18 @@
       <c r="C32">
         <v>945000</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_chicken.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -797,8 +1128,18 @@
       <c r="C33">
         <v>51500</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_cow.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -808,8 +1149,18 @@
       <c r="C34">
         <v>540000</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_cow.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -819,8 +1170,18 @@
       <c r="C35">
         <v>870000</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_cow.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -830,8 +1191,18 @@
       <c r="C36">
         <v>69800</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_mo.pellet_actino_2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -841,8 +1212,18 @@
       <c r="C37">
         <v>90500</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_mo.pellet_actino_3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -852,8 +1233,18 @@
       <c r="C38">
         <v>49000</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_mo.pellet_actino_1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -863,8 +1254,18 @@
       <c r="C39">
         <v>260000</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_compost_actino_2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -874,8 +1275,18 @@
       <c r="C40">
         <v>800000</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_compost_actino_3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -885,8 +1296,18 @@
       <c r="C41">
         <v>520000</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_compost_actino_1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -896,8 +1317,18 @@
       <c r="C42">
         <v>433000</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.legumes_actino_2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -907,8 +1338,18 @@
       <c r="C43">
         <v>445000</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.legumes_actino_3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -918,8 +1359,18 @@
       <c r="C44">
         <v>420000</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>t1_control.legumes_actino_1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -929,8 +1380,18 @@
       <c r="C45" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>time_treatment_actino_2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -940,8 +1401,18 @@
       <c r="C46">
         <v>405000</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control_actino_3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -951,8 +1422,18 @@
       <c r="C47">
         <v>1110000</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control_actino_1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -962,8 +1443,18 @@
       <c r="C48">
         <v>830000</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control_actino_2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -973,8 +1464,18 @@
       <c r="C49">
         <v>630000</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.amf_actino_3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -984,8 +1485,18 @@
       <c r="C50">
         <v>575000</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.amf_actino_1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -995,8 +1506,18 @@
       <c r="C51">
         <v>535000</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.amf_actino_2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1006,8 +1527,18 @@
       <c r="C52">
         <v>5800000</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_chicken.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1017,8 +1548,18 @@
       <c r="C53">
         <v>6300000</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_chicken.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1028,8 +1569,18 @@
       <c r="C54">
         <v>2200000</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_chicken.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1039,8 +1590,18 @@
       <c r="C55">
         <v>1030000</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_cow.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1050,8 +1611,18 @@
       <c r="C56">
         <v>3250000</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_cow.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1061,8 +1632,18 @@
       <c r="C57">
         <v>1080000</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_cow.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1072,8 +1653,18 @@
       <c r="C58">
         <v>1050000</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_mo.pellet_actino_3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1083,8 +1674,18 @@
       <c r="C59">
         <v>4300000</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_mo.pellet_actino_1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1094,8 +1695,18 @@
       <c r="C60">
         <v>2750000</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_mo.pellet_actino_2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1105,8 +1716,18 @@
       <c r="C61">
         <v>1320000</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_compost_actino_3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1116,8 +1737,18 @@
       <c r="C62">
         <v>1160000</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_compost_actino_1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1127,8 +1758,18 @@
       <c r="C63">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_compost_actino_2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1138,8 +1779,18 @@
       <c r="C64">
         <v>1340000</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.legumes_actino_3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1149,8 +1800,18 @@
       <c r="C65">
         <v>2480000</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.legumes_actino_1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1160,8 +1821,18 @@
       <c r="C66">
         <v>3110000</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>t2_control.legumes_actino_2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -1171,8 +1842,18 @@
       <c r="C67" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F88" si="1">A67&amp;"_"&amp;B67&amp;"_"&amp;"actino"&amp;"_"&amp;E67</f>
+        <v>time_treatment_actino_3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1182,8 +1863,18 @@
       <c r="C68">
         <v>955000</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control_actino_1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -1193,8 +1884,18 @@
       <c r="C69">
         <v>390000</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control_actino_2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -1204,8 +1905,18 @@
       <c r="C70">
         <v>595000</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control_actino_3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -1215,8 +1926,18 @@
       <c r="C71">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.amf_actino_1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -1226,8 +1947,18 @@
       <c r="C72">
         <v>555000</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.amf_actino_2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -1237,8 +1968,18 @@
       <c r="C73">
         <v>990000</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.amf_actino_3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -1248,8 +1989,18 @@
       <c r="C74">
         <v>12100000</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_chicken.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -1259,8 +2010,18 @@
       <c r="C75">
         <v>3150000</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_chicken.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +2031,18 @@
       <c r="C76">
         <v>3450000</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_chicken.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -1281,8 +2052,18 @@
       <c r="C77">
         <v>1180000</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D77" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_cow.manure_actino_1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -1292,8 +2073,18 @@
       <c r="C78">
         <v>3250000</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_cow.manure_actino_2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -1303,8 +2094,18 @@
       <c r="C79">
         <v>2900000</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_cow.manure_actino_3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -1314,8 +2115,18 @@
       <c r="C80">
         <v>1070000</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D80" t="s">
+        <v>15</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_mo.pellet_actino_1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -1325,8 +2136,18 @@
       <c r="C81">
         <v>500000</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_mo.pellet_actino_2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -1336,8 +2157,18 @@
       <c r="C82">
         <v>460000</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_mo.pellet_actino_3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -1347,8 +2178,18 @@
       <c r="C83">
         <v>1160000</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D83" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_compost_actino_1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -1358,8 +2199,18 @@
       <c r="C84">
         <v>1150000</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_compost_actino_2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -1369,8 +2220,18 @@
       <c r="C85">
         <v>1030000</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D85" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85">
+        <v>3</v>
+      </c>
+      <c r="F85" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_compost_actino_3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -1380,8 +2241,18 @@
       <c r="C86">
         <v>4800000</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.legumes_actino_1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -1391,8 +2262,18 @@
       <c r="C87">
         <v>2080000</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D87" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.legumes_actino_2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -1401,6 +2282,16 @@
       </c>
       <c r="C88">
         <v>1360000</v>
+      </c>
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" si="1"/>
+        <v>t3_control.legumes_actino_3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more data for PCA training
</commit_message>
<xml_diff>
--- a/raw_files/cfu_actinobacteria.xlsx
+++ b/raw_files/cfu_actinobacteria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.romero\ownCloud - Romero Ignacio@owncloud.fibl.org\exchange_iro_nbo_vgf\iro\banana_microbiome\raw_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55B390-6A6C-4078-B2F7-1A72C189B1A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB726F7-82FD-421A-B187-5C0836A8B8CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{65FEA12C-D4E3-4D9D-BB5A-CCA2AEA21078}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="18">
   <si>
     <t>time</t>
   </si>
@@ -439,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6965D11-17F6-4B89-8430-518B48E14CEB}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="0">A3&amp;"_"&amp;B3&amp;"_"&amp;"actino"&amp;"_"&amp;E3</f>
+        <f t="shared" ref="F3:F64" si="0">A3&amp;"_"&amp;B3&amp;"_"&amp;"actino"&amp;"_"&amp;E3</f>
         <v>t0_control_actino_2</v>
       </c>
     </row>
@@ -910,23 +910,23 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>65000</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>time_treatment_actino_1</v>
+        <v>t1_control_actino_2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -937,17 +937,17 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>65000</v>
+        <v>46500</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control_actino_2</v>
+        <v>t1_control_actino_3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -958,17 +958,17 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>46500</v>
+        <v>83500</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control_actino_3</v>
+        <v>t1_control_actino_1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -976,20 +976,20 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>83500</v>
+        <v>49500</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control_actino_1</v>
+        <v>t1_control.amf_actino_2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1000,17 +1000,17 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>49500</v>
+        <v>53500</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.amf_actino_2</v>
+        <v>t1_control.amf_actino_3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1021,17 +1021,17 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>53500</v>
+        <v>45500</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.amf_actino_3</v>
+        <v>t1_control.amf_actino_1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1039,20 +1039,20 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>45500</v>
+        <v>44500</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.amf_actino_1</v>
+        <v>t1_chicken.manure_actino_2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1063,17 +1063,17 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>44500</v>
+        <v>1400000</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>t1_chicken.manure_actino_2</v>
+        <v>t1_chicken.manure_actino_3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1084,17 +1084,17 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>1400000</v>
+        <v>945000</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>t1_chicken.manure_actino_3</v>
+        <v>t1_chicken.manure_actino_1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1102,20 +1102,20 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>945000</v>
+        <v>51500</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>t1_chicken.manure_actino_1</v>
+        <v>t1_cow.manure_actino_2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1126,17 +1126,17 @@
         <v>11</v>
       </c>
       <c r="C33">
-        <v>51500</v>
+        <v>540000</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>t1_cow.manure_actino_2</v>
+        <v>t1_cow.manure_actino_3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1147,17 +1147,17 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <v>540000</v>
+        <v>870000</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>t1_cow.manure_actino_3</v>
+        <v>t1_cow.manure_actino_1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1165,20 +1165,20 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <v>870000</v>
+        <v>69800</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>t1_cow.manure_actino_1</v>
+        <v>t1_mo.pellet_actino_2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1189,17 +1189,17 @@
         <v>12</v>
       </c>
       <c r="C36">
-        <v>69800</v>
+        <v>90500</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>t1_mo.pellet_actino_2</v>
+        <v>t1_mo.pellet_actino_3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1210,17 +1210,17 @@
         <v>12</v>
       </c>
       <c r="C37">
-        <v>90500</v>
+        <v>49000</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
       </c>
       <c r="E37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>t1_mo.pellet_actino_3</v>
+        <v>t1_mo.pellet_actino_1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1228,20 +1228,20 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>49000</v>
+        <v>260000</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>t1_mo.pellet_actino_1</v>
+        <v>t1_compost_actino_2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1252,17 +1252,17 @@
         <v>4</v>
       </c>
       <c r="C39">
-        <v>260000</v>
+        <v>800000</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>t1_compost_actino_2</v>
+        <v>t1_compost_actino_3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1273,17 +1273,17 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>800000</v>
+        <v>520000</v>
       </c>
       <c r="D40" t="s">
         <v>15</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>t1_compost_actino_3</v>
+        <v>t1_compost_actino_1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1291,20 +1291,20 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C41">
-        <v>520000</v>
+        <v>433000</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>t1_compost_actino_1</v>
+        <v>t1_control.legumes_actino_2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1315,17 +1315,17 @@
         <v>13</v>
       </c>
       <c r="C42">
-        <v>433000</v>
+        <v>445000</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.legumes_actino_2</v>
+        <v>t1_control.legumes_actino_3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1336,59 +1336,59 @@
         <v>13</v>
       </c>
       <c r="C43">
-        <v>445000</v>
+        <v>420000</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
       </c>
       <c r="E43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.legumes_actino_3</v>
+        <v>t1_control.legumes_actino_1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>420000</v>
+        <v>405000</v>
       </c>
       <c r="D44" t="s">
         <v>15</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>t1_control.legumes_actino_1</v>
+        <v>t2_control_actino_3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>1110000</v>
       </c>
       <c r="D45" t="s">
         <v>15</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>time_treatment_actino_2</v>
+        <v>t2_control_actino_1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1399,17 +1399,17 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>405000</v>
+        <v>830000</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control_actino_3</v>
+        <v>t2_control_actino_2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1417,20 +1417,20 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>1110000</v>
+        <v>630000</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control_actino_1</v>
+        <v>t2_control.amf_actino_3</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1438,20 +1438,20 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C48">
-        <v>830000</v>
+        <v>575000</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control_actino_2</v>
+        <v>t2_control.amf_actino_1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1462,17 +1462,17 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>630000</v>
+        <v>535000</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control.amf_actino_3</v>
+        <v>t2_control.amf_actino_2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1480,20 +1480,20 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>575000</v>
+        <v>5800000</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control.amf_actino_1</v>
+        <v>t2_chicken.manure_actino_3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,20 +1501,20 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C51">
-        <v>535000</v>
+        <v>6300000</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control.amf_actino_2</v>
+        <v>t2_chicken.manure_actino_1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1525,17 +1525,17 @@
         <v>10</v>
       </c>
       <c r="C52">
-        <v>5800000</v>
+        <v>2200000</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>t2_chicken.manure_actino_3</v>
+        <v>t2_chicken.manure_actino_2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1543,20 +1543,20 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>6300000</v>
+        <v>1030000</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>t2_chicken.manure_actino_1</v>
+        <v>t2_cow.manure_actino_3</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1564,20 +1564,20 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C54">
-        <v>2200000</v>
+        <v>3250000</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>t2_chicken.manure_actino_2</v>
+        <v>t2_cow.manure_actino_1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,17 +1588,17 @@
         <v>11</v>
       </c>
       <c r="C55">
-        <v>1030000</v>
+        <v>1080000</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>t2_cow.manure_actino_3</v>
+        <v>t2_cow.manure_actino_2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1606,20 +1606,20 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>3250000</v>
+        <v>1050000</v>
       </c>
       <c r="D56" t="s">
         <v>15</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>t2_cow.manure_actino_1</v>
+        <v>t2_mo.pellet_actino_3</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1627,20 +1627,20 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>1080000</v>
+        <v>4300000</v>
       </c>
       <c r="D57" t="s">
         <v>15</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>t2_cow.manure_actino_2</v>
+        <v>t2_mo.pellet_actino_1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,17 +1651,17 @@
         <v>12</v>
       </c>
       <c r="C58">
-        <v>1050000</v>
+        <v>2750000</v>
       </c>
       <c r="D58" t="s">
         <v>15</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>t2_mo.pellet_actino_3</v>
+        <v>t2_mo.pellet_actino_2</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1669,20 +1669,20 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>4300000</v>
+        <v>1320000</v>
       </c>
       <c r="D59" t="s">
         <v>15</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>t2_mo.pellet_actino_1</v>
+        <v>t2_compost_actino_3</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1690,20 +1690,20 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C60">
-        <v>2750000</v>
+        <v>1160000</v>
       </c>
       <c r="D60" t="s">
         <v>15</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>t2_mo.pellet_actino_2</v>
+        <v>t2_compost_actino_1</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1714,17 +1714,17 @@
         <v>4</v>
       </c>
       <c r="C61">
-        <v>1320000</v>
+        <v>1000000</v>
       </c>
       <c r="D61" t="s">
         <v>15</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>t2_compost_actino_3</v>
+        <v>t2_compost_actino_2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,20 +1732,20 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C62">
-        <v>1160000</v>
+        <v>1340000</v>
       </c>
       <c r="D62" t="s">
         <v>15</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>t2_compost_actino_1</v>
+        <v>t2_control.legumes_actino_3</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1753,20 +1753,20 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C63">
-        <v>1000000</v>
+        <v>2480000</v>
       </c>
       <c r="D63" t="s">
         <v>15</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>t2_compost_actino_2</v>
+        <v>t2_control.legumes_actino_1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,28 +1777,28 @@
         <v>13</v>
       </c>
       <c r="C64">
-        <v>1340000</v>
+        <v>3110000</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>t2_control.legumes_actino_3</v>
+        <v>t2_control.legumes_actino_2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>2480000</v>
+        <v>955000</v>
       </c>
       <c r="D65" t="s">
         <v>15</v>
@@ -1807,19 +1807,19 @@
         <v>1</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>t2_control.legumes_actino_1</v>
+        <f t="shared" ref="F65:F85" si="1">A65&amp;"_"&amp;B65&amp;"_"&amp;"actino"&amp;"_"&amp;E65</f>
+        <v>t3_control_actino_1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>3110000</v>
+        <v>390000</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -1828,19 +1828,19 @@
         <v>2</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>t2_control.legumes_actino_2</v>
+        <f t="shared" si="1"/>
+        <v>t3_control_actino_2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>595000</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -1849,8 +1849,8 @@
         <v>3</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F88" si="1">A67&amp;"_"&amp;B67&amp;"_"&amp;"actino"&amp;"_"&amp;E67</f>
-        <v>time_treatment_actino_3</v>
+        <f t="shared" si="1"/>
+        <v>t3_control_actino_3</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1858,10 +1858,10 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>955000</v>
+        <v>1000000</v>
       </c>
       <c r="D68" t="s">
         <v>15</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control_actino_1</v>
+        <v>t3_control.amf_actino_1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -1879,10 +1879,10 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>390000</v>
+        <v>555000</v>
       </c>
       <c r="D69" t="s">
         <v>15</v>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control_actino_2</v>
+        <v>t3_control.amf_actino_2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1900,10 +1900,10 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>595000</v>
+        <v>990000</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control_actino_3</v>
+        <v>t3_control.amf_actino_3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1921,10 +1921,10 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>1000000</v>
+        <v>12100000</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control.amf_actino_1</v>
+        <v>t3_chicken.manure_actino_1</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -1942,10 +1942,10 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>555000</v>
+        <v>3150000</v>
       </c>
       <c r="D72" t="s">
         <v>15</v>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control.amf_actino_2</v>
+        <v>t3_chicken.manure_actino_2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -1963,10 +1963,10 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>990000</v>
+        <v>3450000</v>
       </c>
       <c r="D73" t="s">
         <v>15</v>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v>t3_control.amf_actino_3</v>
+        <v>t3_chicken.manure_actino_3</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1984,10 +1984,10 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>12100000</v>
+        <v>1180000</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v>t3_chicken.manure_actino_1</v>
+        <v>t3_cow.manure_actino_1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2005,10 +2005,10 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>3150000</v>
+        <v>3250000</v>
       </c>
       <c r="D75" t="s">
         <v>15</v>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v>t3_chicken.manure_actino_2</v>
+        <v>t3_cow.manure_actino_2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2026,10 +2026,10 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C76">
-        <v>3450000</v>
+        <v>2900000</v>
       </c>
       <c r="D76" t="s">
         <v>15</v>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v>t3_chicken.manure_actino_3</v>
+        <v>t3_cow.manure_actino_3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2047,10 +2047,10 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C77">
-        <v>1180000</v>
+        <v>1070000</v>
       </c>
       <c r="D77" t="s">
         <v>15</v>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v>t3_cow.manure_actino_1</v>
+        <v>t3_mo.pellet_actino_1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2068,10 +2068,10 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C78">
-        <v>3250000</v>
+        <v>500000</v>
       </c>
       <c r="D78" t="s">
         <v>15</v>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v>t3_cow.manure_actino_2</v>
+        <v>t3_mo.pellet_actino_2</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2089,10 +2089,10 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C79">
-        <v>2900000</v>
+        <v>460000</v>
       </c>
       <c r="D79" t="s">
         <v>15</v>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v>t3_cow.manure_actino_3</v>
+        <v>t3_mo.pellet_actino_3</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2110,10 +2110,10 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>1070000</v>
+        <v>1160000</v>
       </c>
       <c r="D80" t="s">
         <v>15</v>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v>t3_mo.pellet_actino_1</v>
+        <v>t3_compost_actino_1</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2131,10 +2131,10 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C81">
-        <v>500000</v>
+        <v>1150000</v>
       </c>
       <c r="D81" t="s">
         <v>15</v>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v>t3_mo.pellet_actino_2</v>
+        <v>t3_compost_actino_2</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2152,10 +2152,10 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C82">
-        <v>460000</v>
+        <v>1030000</v>
       </c>
       <c r="D82" t="s">
         <v>15</v>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v>t3_mo.pellet_actino_3</v>
+        <v>t3_compost_actino_3</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,10 +2173,10 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C83">
-        <v>1160000</v>
+        <v>4800000</v>
       </c>
       <c r="D83" t="s">
         <v>15</v>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v>t3_compost_actino_1</v>
+        <v>t3_control.legumes_actino_1</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2194,10 +2194,10 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C84">
-        <v>1150000</v>
+        <v>2080000</v>
       </c>
       <c r="D84" t="s">
         <v>15</v>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v>t3_compost_actino_2</v>
+        <v>t3_control.legumes_actino_2</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2215,10 +2215,10 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C85">
-        <v>1030000</v>
+        <v>1360000</v>
       </c>
       <c r="D85" t="s">
         <v>15</v>
@@ -2227,69 +2227,6 @@
         <v>3</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="1"/>
-        <v>t3_compost_actino_3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" t="s">
-        <v>13</v>
-      </c>
-      <c r="C86">
-        <v>4800000</v>
-      </c>
-      <c r="D86" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86">
-        <v>1</v>
-      </c>
-      <c r="F86" t="str">
-        <f t="shared" si="1"/>
-        <v>t3_control.legumes_actino_1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>7</v>
-      </c>
-      <c r="B87" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87">
-        <v>2080000</v>
-      </c>
-      <c r="D87" t="s">
-        <v>15</v>
-      </c>
-      <c r="E87">
-        <v>2</v>
-      </c>
-      <c r="F87" t="str">
-        <f t="shared" si="1"/>
-        <v>t3_control.legumes_actino_2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88">
-        <v>1360000</v>
-      </c>
-      <c r="D88" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88">
-        <v>3</v>
-      </c>
-      <c r="F88" t="str">
         <f t="shared" si="1"/>
         <v>t3_control.legumes_actino_3</v>
       </c>

</xml_diff>